<commit_message>
enhancement for payroll page for monthly frequency completed
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioThree201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioThree201718.xlsx
@@ -1,76 +1,76 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="30" windowWidth="15165" windowHeight="5400" firstSheet="40" activeTab="40"/>
+    <workbookView activeTab="40" firstSheet="40" windowHeight="5400" windowWidth="15165" xWindow="390" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="ResetEmployeeData" sheetId="14" r:id="rId2"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM1" sheetId="6" r:id="rId3"/>
-    <sheet name="ProcessPayrollForApril" sheetId="7" r:id="rId4"/>
-    <sheet name="ProcessFinalPayrollForApril" sheetId="49" r:id="rId5"/>
-    <sheet name="TestAprilReports" sheetId="11" r:id="rId6"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM2" sheetId="15" r:id="rId7"/>
-    <sheet name="ProcessPayrollForMay" sheetId="16" r:id="rId8"/>
-    <sheet name="ProcessFinalPayrollForMay" sheetId="17" r:id="rId9"/>
-    <sheet name="TestMayReports" sheetId="18" r:id="rId10"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM3" sheetId="51" r:id="rId11"/>
-    <sheet name="ProcessPayrollForJune" sheetId="19" r:id="rId12"/>
-    <sheet name="ProcessFinalPayrollForJune" sheetId="50" r:id="rId13"/>
-    <sheet name="TestJuneReports" sheetId="20" r:id="rId14"/>
-    <sheet name="ResetEmployeeDataJuly" sheetId="61" r:id="rId15"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM4" sheetId="21" r:id="rId16"/>
-    <sheet name="ProcessPayrollForJuly" sheetId="22" r:id="rId17"/>
-    <sheet name="ProcessFinalPayrollForJuly" sheetId="52" r:id="rId18"/>
-    <sheet name="TestJulyReports" sheetId="23" r:id="rId19"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM5" sheetId="24" r:id="rId20"/>
-    <sheet name="ProcessPayrollForAug" sheetId="25" r:id="rId21"/>
-    <sheet name="ProcessFinalPayrollForAug" sheetId="53" r:id="rId22"/>
-    <sheet name="TestAugReports" sheetId="26" r:id="rId23"/>
-    <sheet name="ResetEmployeeDataSep" sheetId="63" r:id="rId24"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM6" sheetId="27" r:id="rId25"/>
-    <sheet name="ProcessPayrollForSep" sheetId="28" r:id="rId26"/>
-    <sheet name="ProcessFinalPayrollForSep" sheetId="54" r:id="rId27"/>
-    <sheet name="TestSepReports" sheetId="29" r:id="rId28"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM7" sheetId="30" r:id="rId29"/>
-    <sheet name="ProcessPayrollForOct" sheetId="31" r:id="rId30"/>
-    <sheet name="ProcessFinalPayrollForOct" sheetId="55" r:id="rId31"/>
-    <sheet name="TestOctReports" sheetId="32" r:id="rId32"/>
-    <sheet name="ResetEmployeeDataNov" sheetId="64" r:id="rId33"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM8" sheetId="33" r:id="rId34"/>
-    <sheet name="ProcessPayrollForNov" sheetId="34" r:id="rId35"/>
-    <sheet name="ProcessFinalPayrollForNov" sheetId="56" r:id="rId36"/>
-    <sheet name="TestNovReports" sheetId="35" r:id="rId37"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM9" sheetId="36" r:id="rId38"/>
-    <sheet name="ProcessPayrollForDec" sheetId="37" r:id="rId39"/>
-    <sheet name="ProcessFinalPayrollForDec" sheetId="57" r:id="rId40"/>
-    <sheet name="TestDecReports" sheetId="38" r:id="rId41"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM10" sheetId="39" r:id="rId42"/>
-    <sheet name="ProcessPayrollForJan" sheetId="40" r:id="rId43"/>
-    <sheet name="ProcessFinalPayrollForJan" sheetId="58" r:id="rId44"/>
-    <sheet name="TestJanReports" sheetId="41" r:id="rId45"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM11" sheetId="42" r:id="rId46"/>
-    <sheet name="ProcessPayrollForFeb" sheetId="43" r:id="rId47"/>
-    <sheet name="ProcessFinalPayrollForFeb" sheetId="59" r:id="rId48"/>
-    <sheet name="TestFebReports" sheetId="44" r:id="rId49"/>
-    <sheet name="ProcessPayrollForMarch" sheetId="46" r:id="rId50"/>
-    <sheet name="ProcessFinalPayrollForMarch" sheetId="60" r:id="rId51"/>
-    <sheet name="TestMarchReports" sheetId="47" r:id="rId52"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="ResetEmployeeData" r:id="rId2" sheetId="14"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM1" r:id="rId3" sheetId="6"/>
+    <sheet name="ProcessPayrollForApril" r:id="rId4" sheetId="7"/>
+    <sheet name="ProcessFinalPayrollForApril" r:id="rId5" sheetId="49"/>
+    <sheet name="TestAprilReports" r:id="rId6" sheetId="11"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM2" r:id="rId7" sheetId="15"/>
+    <sheet name="ProcessPayrollForMay" r:id="rId8" sheetId="16"/>
+    <sheet name="ProcessFinalPayrollForMay" r:id="rId9" sheetId="17"/>
+    <sheet name="TestMayReports" r:id="rId10" sheetId="18"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM3" r:id="rId11" sheetId="51"/>
+    <sheet name="ProcessPayrollForJune" r:id="rId12" sheetId="19"/>
+    <sheet name="ProcessFinalPayrollForJune" r:id="rId13" sheetId="50"/>
+    <sheet name="TestJuneReports" r:id="rId14" sheetId="20"/>
+    <sheet name="ResetEmployeeDataJuly" r:id="rId15" sheetId="61"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM4" r:id="rId16" sheetId="21"/>
+    <sheet name="ProcessPayrollForJuly" r:id="rId17" sheetId="22"/>
+    <sheet name="ProcessFinalPayrollForJuly" r:id="rId18" sheetId="52"/>
+    <sheet name="TestJulyReports" r:id="rId19" sheetId="23"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM5" r:id="rId20" sheetId="24"/>
+    <sheet name="ProcessPayrollForAug" r:id="rId21" sheetId="25"/>
+    <sheet name="ProcessFinalPayrollForAug" r:id="rId22" sheetId="53"/>
+    <sheet name="TestAugReports" r:id="rId23" sheetId="26"/>
+    <sheet name="ResetEmployeeDataSep" r:id="rId24" sheetId="63"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM6" r:id="rId25" sheetId="27"/>
+    <sheet name="ProcessPayrollForSep" r:id="rId26" sheetId="28"/>
+    <sheet name="ProcessFinalPayrollForSep" r:id="rId27" sheetId="54"/>
+    <sheet name="TestSepReports" r:id="rId28" sheetId="29"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM7" r:id="rId29" sheetId="30"/>
+    <sheet name="ProcessPayrollForOct" r:id="rId30" sheetId="31"/>
+    <sheet name="ProcessFinalPayrollForOct" r:id="rId31" sheetId="55"/>
+    <sheet name="TestOctReports" r:id="rId32" sheetId="32"/>
+    <sheet name="ResetEmployeeDataNov" r:id="rId33" sheetId="64"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM8" r:id="rId34" sheetId="33"/>
+    <sheet name="ProcessPayrollForNov" r:id="rId35" sheetId="34"/>
+    <sheet name="ProcessFinalPayrollForNov" r:id="rId36" sheetId="56"/>
+    <sheet name="TestNovReports" r:id="rId37" sheetId="35"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM9" r:id="rId38" sheetId="36"/>
+    <sheet name="ProcessPayrollForDec" r:id="rId39" sheetId="37"/>
+    <sheet name="ProcessFinalPayrollForDec" r:id="rId40" sheetId="57"/>
+    <sheet name="TestDecReports" r:id="rId41" sheetId="38"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM10" r:id="rId42" sheetId="39"/>
+    <sheet name="ProcessPayrollForJan" r:id="rId43" sheetId="40"/>
+    <sheet name="ProcessFinalPayrollForJan" r:id="rId44" sheetId="58"/>
+    <sheet name="TestJanReports" r:id="rId45" sheetId="41"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM11" r:id="rId46" sheetId="42"/>
+    <sheet name="ProcessPayrollForFeb" r:id="rId47" sheetId="43"/>
+    <sheet name="ProcessFinalPayrollForFeb" r:id="rId48" sheetId="59"/>
+    <sheet name="TestFebReports" r:id="rId49" sheetId="44"/>
+    <sheet name="ProcessPayrollForMarch" r:id="rId50" sheetId="46"/>
+    <sheet name="ProcessFinalPayrollForMarch" r:id="rId51" sheetId="60"/>
+    <sheet name="TestMarchReports" r:id="rId52" sheetId="47"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="201">
   <si>
     <t>TC</t>
   </si>
@@ -680,6 +680,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -739,64 +740,64 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -813,10 +814,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -851,7 +852,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -903,7 +904,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1008,7 +1009,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1017,13 +1018,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1033,7 +1034,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1042,7 +1043,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1051,7 +1052,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1061,12 +1062,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1097,7 +1098,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1116,7 +1117,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1128,7 +1129,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
@@ -1137,10 +1138,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1895,12 +1896,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
@@ -1909,22 +1910,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="27" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="20.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1977,7 +1978,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="10" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -2026,15 +2027,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2043,12 +2044,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2080,7 +2081,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>161</v>
       </c>
@@ -2104,12 +2105,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -2118,19 +2119,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="51.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.85546875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="51.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2177,7 +2178,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="78" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -2219,14 +2220,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -2235,17 +2236,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="49.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="49.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2292,7 +2293,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="56.25" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -2334,14 +2335,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -2350,23 +2351,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="6.5703125" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="6.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="6.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -2419,7 +2420,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="10" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -2468,14 +2469,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2484,14 +2485,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="9.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -2529,7 +2530,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>161</v>
       </c>
@@ -2563,12 +2564,12 @@
       <c r="M2" s="10"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2577,12 +2578,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2614,7 +2615,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>161</v>
       </c>
@@ -2638,12 +2639,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -2652,18 +2653,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2710,7 +2711,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="80.25" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -2752,14 +2753,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -2768,16 +2769,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="52.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="52.7109375" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="25.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2824,7 +2825,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="57" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -2866,14 +2867,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -2882,23 +2883,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.85546875" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="5.85546875" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="5.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="5.85546875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="5.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -2951,7 +2952,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="10" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="71.25" r="2" s="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -3000,14 +3001,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3016,19 +3017,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="59" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="22.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="59.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -3072,7 +3073,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>161</v>
       </c>
@@ -3112,13 +3113,13 @@
       <c r="O2" s="10"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3127,13 +3128,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="49.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3165,7 +3166,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>161</v>
       </c>
@@ -3189,12 +3190,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -3203,18 +3204,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="40.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="39.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="53.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="53.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3261,7 +3262,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="62.25" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -3303,14 +3304,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -3319,14 +3320,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="22.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3373,7 +3374,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -3415,14 +3416,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -3431,23 +3432,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.42578125" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="6.28515625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="6.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="6.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -3500,7 +3501,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="10" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -3549,14 +3550,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3565,10 +3566,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="36.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3591,7 +3592,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>161</v>
       </c>
@@ -3606,13 +3607,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3621,12 +3622,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3658,7 +3659,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>161</v>
       </c>
@@ -3682,12 +3683,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -3696,20 +3697,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="43.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3756,7 +3757,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -3798,14 +3799,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -3814,16 +3815,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="44.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3870,7 +3871,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="53.25" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -3912,14 +3913,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -3928,20 +3929,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="38.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="38.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="21.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -3994,7 +3995,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="10" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -4043,14 +4044,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4059,12 +4060,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -4096,7 +4097,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>161</v>
       </c>
@@ -4120,12 +4121,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4134,10 +4135,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="59.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="59.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -4169,7 +4170,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>161</v>
       </c>
@@ -4193,13 +4194,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -4208,20 +4209,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="52.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.28515625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="52.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4268,7 +4269,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -4310,14 +4311,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -4326,17 +4327,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4383,7 +4384,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -4425,14 +4426,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -4441,21 +4442,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="23.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -4508,7 +4509,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="10" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -4557,14 +4558,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4573,9 +4574,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="40.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -4598,7 +4599,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>161</v>
       </c>
@@ -4613,13 +4614,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4628,13 +4629,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -4666,7 +4667,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>161</v>
       </c>
@@ -4690,12 +4691,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
@@ -4704,18 +4705,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4762,7 +4763,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -4804,14 +4805,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -4820,14 +4821,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="32" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4874,7 +4875,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -4916,14 +4917,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -4932,21 +4933,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="11.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -4999,7 +5000,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="10" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -5048,14 +5049,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5064,13 +5065,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="40.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="48.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="40.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -5102,7 +5103,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="10" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="40.9" r="2" s="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>161</v>
       </c>
@@ -5126,13 +5127,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -5141,18 +5142,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5199,7 +5200,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -5241,14 +5242,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -5257,18 +5258,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5315,7 +5316,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="6" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>82</v>
       </c>
@@ -5355,15 +5356,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -5372,15 +5373,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.7109375" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="21.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5427,7 +5428,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -5469,14 +5470,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
@@ -5485,21 +5486,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -5552,7 +5553,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="10" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -5601,14 +5602,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -5617,12 +5618,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="47.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="47.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -5654,7 +5655,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="10" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="40.9" r="2" s="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>161</v>
       </c>
@@ -5678,13 +5679,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -5693,18 +5694,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5751,7 +5752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -5793,14 +5794,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -5809,13 +5810,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5862,7 +5863,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -5904,14 +5905,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -5920,21 +5921,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -5987,7 +5988,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="10" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -6036,15 +6037,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6053,15 +6054,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="6.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="47.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="5.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="6.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6093,7 +6094,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="10" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="40.9" r="2" s="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>161</v>
       </c>
@@ -6117,12 +6118,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -6131,18 +6132,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -6189,7 +6190,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -6231,14 +6232,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -6247,14 +6248,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -6301,7 +6302,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -6343,14 +6344,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -6359,20 +6360,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -6425,7 +6426,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="10" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -6474,14 +6475,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -6490,18 +6491,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="41.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="41.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -6548,7 +6549,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="6" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>82</v>
       </c>
@@ -6588,14 +6589,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6604,18 +6605,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -6662,7 +6663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -6704,16 +6705,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
-    <hyperlink ref="E2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a1Fb0000007GFbv"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000007GFbv" r:id="rId2" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId3" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6722,18 +6723,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="43.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -6780,7 +6781,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -6822,15 +6823,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
-    <hyperlink ref="E2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a1Fb0000007GFbv"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000007GFbv" r:id="rId2" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -6839,20 +6840,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="38.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" width="16.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -6905,7 +6906,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="10" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -6954,16 +6955,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
-    <hyperlink ref="E2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a1Fb0000007GFbv"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000007GFbv" r:id="rId2" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId3" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -6972,23 +6973,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="32.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="18.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="1" s="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>16</v>
       </c>
@@ -7041,7 +7042,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="10" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -7090,15 +7091,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7107,12 +7108,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="47.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -7144,7 +7145,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>161</v>
       </c>
@@ -7168,13 +7169,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -7183,18 +7184,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -7241,7 +7242,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="57" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -7283,14 +7284,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -7299,18 +7300,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -7357,7 +7358,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="51" r="2" s="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -7399,8 +7400,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pagination Code checkin RTI Scenario3
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioThree201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioThree201718.xlsx
@@ -4,68 +4,68 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="396" yWindow="36" windowWidth="15168" windowHeight="5400" firstSheet="48" activeTab="51"/>
+    <workbookView activeTab="51" firstSheet="48" windowHeight="5400" windowWidth="15168" xWindow="396" yWindow="36"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="ResetEmployeeData" sheetId="14" r:id="rId2"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM1" sheetId="6" r:id="rId3"/>
-    <sheet name="ProcessPayrollForApril" sheetId="7" r:id="rId4"/>
-    <sheet name="ProcessFinalPayrollForApril" sheetId="49" r:id="rId5"/>
-    <sheet name="TestAprilReports" sheetId="11" r:id="rId6"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM2" sheetId="15" r:id="rId7"/>
-    <sheet name="ProcessPayrollForMay" sheetId="16" r:id="rId8"/>
-    <sheet name="ProcessFinalPayrollForMay" sheetId="17" r:id="rId9"/>
-    <sheet name="TestMayReports" sheetId="18" r:id="rId10"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM3" sheetId="51" r:id="rId11"/>
-    <sheet name="ProcessPayrollForJune" sheetId="19" r:id="rId12"/>
-    <sheet name="ProcessFinalPayrollForJune" sheetId="50" r:id="rId13"/>
-    <sheet name="TestJuneReports" sheetId="20" r:id="rId14"/>
-    <sheet name="ResetEmployeeDataJuly" sheetId="61" r:id="rId15"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM4" sheetId="21" r:id="rId16"/>
-    <sheet name="ProcessPayrollForJuly" sheetId="22" r:id="rId17"/>
-    <sheet name="ProcessFinalPayrollForJuly" sheetId="52" r:id="rId18"/>
-    <sheet name="TestJulyReports" sheetId="23" r:id="rId19"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM5" sheetId="24" r:id="rId20"/>
-    <sheet name="ProcessPayrollForAug" sheetId="25" r:id="rId21"/>
-    <sheet name="ProcessFinalPayrollForAug" sheetId="53" r:id="rId22"/>
-    <sheet name="TestAugReports" sheetId="26" r:id="rId23"/>
-    <sheet name="ResetEmployeeDataSep" sheetId="63" r:id="rId24"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM6" sheetId="27" r:id="rId25"/>
-    <sheet name="ProcessPayrollForSep" sheetId="28" r:id="rId26"/>
-    <sheet name="ProcessFinalPayrollForSep" sheetId="54" r:id="rId27"/>
-    <sheet name="TestSepReports" sheetId="29" r:id="rId28"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM7" sheetId="30" r:id="rId29"/>
-    <sheet name="ProcessPayrollForOct" sheetId="31" r:id="rId30"/>
-    <sheet name="ProcessFinalPayrollForOct" sheetId="55" r:id="rId31"/>
-    <sheet name="TestOctReports" sheetId="32" r:id="rId32"/>
-    <sheet name="ResetEmployeeDataNov" sheetId="64" r:id="rId33"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM8" sheetId="33" r:id="rId34"/>
-    <sheet name="ProcessPayrollForNov" sheetId="34" r:id="rId35"/>
-    <sheet name="ProcessFinalPayrollForNov" sheetId="56" r:id="rId36"/>
-    <sheet name="TestNovReports" sheetId="35" r:id="rId37"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM9" sheetId="36" r:id="rId38"/>
-    <sheet name="ProcessPayrollForDec" sheetId="37" r:id="rId39"/>
-    <sheet name="ProcessFinalPayrollForDec" sheetId="57" r:id="rId40"/>
-    <sheet name="TestDecReports" sheetId="38" r:id="rId41"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM10" sheetId="39" r:id="rId42"/>
-    <sheet name="ProcessPayrollForJan" sheetId="40" r:id="rId43"/>
-    <sheet name="ProcessFinalPayrollForJan" sheetId="58" r:id="rId44"/>
-    <sheet name="TestJanReports" sheetId="41" r:id="rId45"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM11" sheetId="42" r:id="rId46"/>
-    <sheet name="ProcessPayrollForFeb" sheetId="43" r:id="rId47"/>
-    <sheet name="ProcessFinalPayrollForFeb" sheetId="59" r:id="rId48"/>
-    <sheet name="TestFebReports" sheetId="44" r:id="rId49"/>
-    <sheet name="ProcessPayrollForMarch" sheetId="46" r:id="rId50"/>
-    <sheet name="ProcessFinalPayrollForMarch" sheetId="60" r:id="rId51"/>
-    <sheet name="TestMarchReports" sheetId="47" r:id="rId52"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="ResetEmployeeData" r:id="rId2" sheetId="14"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM1" r:id="rId3" sheetId="6"/>
+    <sheet name="ProcessPayrollForApril" r:id="rId4" sheetId="7"/>
+    <sheet name="ProcessFinalPayrollForApril" r:id="rId5" sheetId="49"/>
+    <sheet name="TestAprilReports" r:id="rId6" sheetId="11"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM2" r:id="rId7" sheetId="15"/>
+    <sheet name="ProcessPayrollForMay" r:id="rId8" sheetId="16"/>
+    <sheet name="ProcessFinalPayrollForMay" r:id="rId9" sheetId="17"/>
+    <sheet name="TestMayReports" r:id="rId10" sheetId="18"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM3" r:id="rId11" sheetId="51"/>
+    <sheet name="ProcessPayrollForJune" r:id="rId12" sheetId="19"/>
+    <sheet name="ProcessFinalPayrollForJune" r:id="rId13" sheetId="50"/>
+    <sheet name="TestJuneReports" r:id="rId14" sheetId="20"/>
+    <sheet name="ResetEmployeeDataJuly" r:id="rId15" sheetId="61"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM4" r:id="rId16" sheetId="21"/>
+    <sheet name="ProcessPayrollForJuly" r:id="rId17" sheetId="22"/>
+    <sheet name="ProcessFinalPayrollForJuly" r:id="rId18" sheetId="52"/>
+    <sheet name="TestJulyReports" r:id="rId19" sheetId="23"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM5" r:id="rId20" sheetId="24"/>
+    <sheet name="ProcessPayrollForAug" r:id="rId21" sheetId="25"/>
+    <sheet name="ProcessFinalPayrollForAug" r:id="rId22" sheetId="53"/>
+    <sheet name="TestAugReports" r:id="rId23" sheetId="26"/>
+    <sheet name="ResetEmployeeDataSep" r:id="rId24" sheetId="63"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM6" r:id="rId25" sheetId="27"/>
+    <sheet name="ProcessPayrollForSep" r:id="rId26" sheetId="28"/>
+    <sheet name="ProcessFinalPayrollForSep" r:id="rId27" sheetId="54"/>
+    <sheet name="TestSepReports" r:id="rId28" sheetId="29"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM7" r:id="rId29" sheetId="30"/>
+    <sheet name="ProcessPayrollForOct" r:id="rId30" sheetId="31"/>
+    <sheet name="ProcessFinalPayrollForOct" r:id="rId31" sheetId="55"/>
+    <sheet name="TestOctReports" r:id="rId32" sheetId="32"/>
+    <sheet name="ResetEmployeeDataNov" r:id="rId33" sheetId="64"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM8" r:id="rId34" sheetId="33"/>
+    <sheet name="ProcessPayrollForNov" r:id="rId35" sheetId="34"/>
+    <sheet name="ProcessFinalPayrollForNov" r:id="rId36" sheetId="56"/>
+    <sheet name="TestNovReports" r:id="rId37" sheetId="35"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM9" r:id="rId38" sheetId="36"/>
+    <sheet name="ProcessPayrollForDec" r:id="rId39" sheetId="37"/>
+    <sheet name="ProcessFinalPayrollForDec" r:id="rId40" sheetId="57"/>
+    <sheet name="TestDecReports" r:id="rId41" sheetId="38"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM10" r:id="rId42" sheetId="39"/>
+    <sheet name="ProcessPayrollForJan" r:id="rId43" sheetId="40"/>
+    <sheet name="ProcessFinalPayrollForJan" r:id="rId44" sheetId="58"/>
+    <sheet name="TestJanReports" r:id="rId45" sheetId="41"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM11" r:id="rId46" sheetId="42"/>
+    <sheet name="ProcessPayrollForFeb" r:id="rId47" sheetId="43"/>
+    <sheet name="ProcessFinalPayrollForFeb" r:id="rId48" sheetId="59"/>
+    <sheet name="TestFebReports" r:id="rId49" sheetId="44"/>
+    <sheet name="ProcessPayrollForMarch" r:id="rId50" sheetId="46"/>
+    <sheet name="ProcessFinalPayrollForMarch" r:id="rId51" sheetId="60"/>
+    <sheet name="TestMarchReports" r:id="rId52" sheetId="47"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1468" uniqueCount="201">
   <si>
     <t>TC</t>
   </si>
@@ -675,6 +675,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -734,64 +735,64 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -808,10 +809,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -969,7 +970,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -978,13 +979,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -994,7 +995,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1003,7 +1004,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1012,7 +1013,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1022,12 +1023,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1058,7 +1059,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1077,7 +1078,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1089,7 +1090,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
@@ -1098,10 +1099,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1856,12 +1857,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1870,22 +1871,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="27" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="21.6640625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="25.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="21.6640625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="20.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1938,7 +1939,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -1987,15 +1988,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2004,15 +2005,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -2041,7 +2042,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
@@ -2065,12 +2066,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2079,22 +2080,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="51.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.88671875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="31.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="51.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -2138,7 +2139,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="78" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -2180,14 +2181,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2196,20 +2197,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="49.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="42.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="49.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -2253,7 +2254,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="56.25" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -2295,14 +2296,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2311,23 +2312,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.44140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22.6640625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="6.5546875" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="6.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="6.5546875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="6.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -2380,7 +2381,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -2429,14 +2430,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2445,17 +2446,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="9.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -2490,7 +2491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
@@ -2524,12 +2525,12 @@
       <c r="M2" s="9"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2538,15 +2539,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -2575,7 +2576,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
@@ -2599,12 +2600,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2613,21 +2614,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.88671875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -2671,7 +2672,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="80.25" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -2713,14 +2714,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2729,19 +2730,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="52.6640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="52.6640625" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="25.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -2785,7 +2786,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="57" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -2827,14 +2828,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2843,23 +2844,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="21.6640625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.88671875" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="5.88671875" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="5.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="21.6640625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="9.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="5.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="5.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -2912,7 +2913,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="9" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="71.25" r="2" s="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -2961,14 +2962,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2977,22 +2978,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="59" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="22.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.33203125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="8.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="59.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.5546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="22.109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="9.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="6.33203125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -3033,7 +3034,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
@@ -3073,13 +3074,13 @@
       <c r="O2" s="9"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3088,16 +3089,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="49.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -3126,7 +3127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
@@ -3150,12 +3151,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3164,21 +3165,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="40.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="39.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="53.109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="40.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="39.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="53.109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -3222,7 +3223,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="62.25" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -3264,14 +3265,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3280,17 +3281,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.88671875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48.6640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="22.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="23.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="22.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -3334,7 +3335,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -3376,14 +3377,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3392,23 +3393,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22.33203125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.44140625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="6.33203125" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="6.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="26.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="9.44140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="6.33203125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="6.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -3461,7 +3462,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -3510,14 +3511,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3526,13 +3527,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="36.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -3552,7 +3553,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
@@ -3567,13 +3568,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3582,15 +3583,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="9.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -3619,7 +3620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
@@ -3643,12 +3644,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3657,23 +3658,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="43.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.33203125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.6640625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.6640625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.5546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -3717,7 +3718,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -3759,14 +3760,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3775,19 +3776,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="44.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -3831,7 +3832,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="53.25" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -3873,14 +3874,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3889,20 +3890,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.88671875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="38.6640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="21.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="38.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="21.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -3955,7 +3956,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="9" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -4004,14 +4005,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4020,15 +4021,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -4057,7 +4058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
@@ -4081,12 +4082,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4095,13 +4096,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="59.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="59.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -4130,7 +4131,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
@@ -4154,13 +4155,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4169,23 +4170,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="52.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.33203125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.33203125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.33203125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="52.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.33203125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.33203125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -4229,7 +4230,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -4271,14 +4272,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4287,20 +4288,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -4344,7 +4345,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -4386,14 +4387,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4402,21 +4403,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="23.6640625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.5546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -4469,7 +4470,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="9" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -4518,14 +4519,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4534,12 +4535,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="40.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="40.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -4559,7 +4560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
@@ -4574,13 +4575,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4589,16 +4590,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="45.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="9.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -4627,7 +4628,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
@@ -4651,12 +4652,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4665,21 +4666,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48.109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="31.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="21.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.5546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -4723,7 +4724,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -4765,14 +4766,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4781,17 +4782,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="32" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -4835,7 +4836,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -4877,14 +4878,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4893,21 +4894,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.88671875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="11.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -4960,7 +4961,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="9" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -5009,14 +5010,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5025,16 +5026,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="40.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="48.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="40.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -5063,7 +5064,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="9" customFormat="1" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="40.950000000000003" r="2" s="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
@@ -5087,13 +5088,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5102,21 +5103,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.44140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.44140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -5160,7 +5161,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -5202,14 +5203,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5218,18 +5219,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.5546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -5276,7 +5277,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="6" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -5315,13 +5316,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5330,18 +5331,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.6640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.6640625" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="21.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -5385,7 +5386,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -5427,14 +5428,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5443,21 +5444,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.88671875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.5546875" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="12.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -5510,7 +5511,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="9" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -5559,14 +5560,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -5575,15 +5576,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="47.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="47.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -5612,7 +5613,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="9" customFormat="1" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="40.950000000000003" r="2" s="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
@@ -5636,13 +5637,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5651,21 +5652,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.44140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -5709,7 +5710,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -5751,14 +5752,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5767,16 +5768,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -5820,7 +5821,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -5862,14 +5863,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5878,21 +5879,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24.33203125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.33203125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="12.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -5945,7 +5946,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="9" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -5994,15 +5995,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6011,18 +6012,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="6.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="47.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="5.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="6.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -6051,7 +6052,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="9" customFormat="1" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="40.950000000000003" r="2" s="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
@@ -6075,12 +6076,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6089,21 +6090,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.88671875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.88671875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -6147,7 +6148,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -6189,14 +6190,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6205,17 +6206,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -6259,7 +6260,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -6301,14 +6302,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6317,20 +6318,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -6383,7 +6384,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="9" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -6432,14 +6433,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6448,21 +6449,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="41.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.33203125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="41.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -6506,7 +6507,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="6" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -6546,14 +6547,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6562,21 +6563,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.33203125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="42.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.5546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.44140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -6620,7 +6621,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -6662,16 +6663,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000007GFbv"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000007GFbv" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId3" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6680,21 +6681,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="43.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.5546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -6738,7 +6739,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -6780,15 +6781,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000007GFbv"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000007GFbv" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -6797,20 +6798,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.44140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="21.88671875" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="16.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="38.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="26.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="20.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.44140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="21.88671875" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" width="16.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -6863,7 +6864,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="9" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -6912,16 +6913,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a1Fb0000007GFbv"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000007GFbv" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId3" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6930,23 +6931,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="32.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="21.109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="47.44140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="21.109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="18.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="1" s="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>16</v>
       </c>
@@ -6999,7 +7000,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -7048,15 +7049,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7065,15 +7066,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="47.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -7102,7 +7103,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
@@ -7126,13 +7127,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7141,21 +7142,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -7199,7 +7200,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="57" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -7241,14 +7242,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7257,21 +7258,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.88671875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.88671875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -7315,7 +7316,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="51" r="2" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>199</v>
       </c>
@@ -7357,8 +7358,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>